<commit_message>
Update sign-ups, Yonghui, Anna, Ashish
</commit_message>
<xml_diff>
--- a/roles_BioHackathon2023.xlsx
+++ b/roles_BioHackathon2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sjcrh-my.sharepoint.com/personal/sselukar_stjude_org/Documents/Documents/Research/Projects/Methods/TimeVaryingBMT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{B41E7AF5-1FE9-486D-A35E-51493A8912CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B744D17-0518-4D38-B982-D37F2C6AE88E}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{B41E7AF5-1FE9-486D-A35E-51493A8912CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C9E3071-C41F-43DE-AEB5-E91003B1D669}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{28D3244B-B5EB-47D8-A71B-EB5C60FB438C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Front end</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Develop Shiny app: accept user input data and user input covariate trajectory, produce Cox PH summary table and predicted survival curve</t>
+  </si>
+  <si>
+    <t>Yonghui</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Ashish</t>
   </si>
 </sst>
 </file>
@@ -453,7 +462,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,16 +529,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>

</xml_diff>